<commit_message>
Reverse complement and rotation issues
</commit_message>
<xml_diff>
--- a/tabular/core/cress-refseqs-side-data.xlsx
+++ b/tabular/core/cress-refseqs-side-data.xlsx
@@ -1,34 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770AB2A0-CD2D-4E44-8F3B-C9B8371AB461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="1580" windowWidth="36380" windowHeight="20160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9980" yWindow="1580" windowWidth="36380" windowHeight="20160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="196">
   <si>
     <t>PCV-1</t>
   </si>
@@ -481,9 +475,6 @@
   </si>
   <si>
     <t>KJ641714</t>
-  </si>
-  <si>
-    <t>Cyclovirus-3</t>
   </si>
   <si>
     <t>Bat circovirus isolate BtRp-CV-14/GD2012</t>
@@ -624,7 +615,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -763,7 +754,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="316">
+  <cellStyleXfs count="330">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -963,6 +954,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1100,7 +1105,7 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="316">
+  <cellStyles count="330">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1263,6 +1268,13 @@
     <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1416,6 +1428,13 @@
     <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1752,14 +1771,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" style="2" customWidth="1"/>
@@ -1771,9 +1790,9 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>58</v>
@@ -1782,7 +1801,7 @@
         <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>60</v>
@@ -1791,13 +1810,13 @@
         <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
         <v>26</v>
       </c>
@@ -1808,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>2</v>
@@ -1817,13 +1836,13 @@
         <v>53</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>146</v>
       </c>
@@ -1834,7 +1853,7 @@
         <v>147</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>2</v>
@@ -1843,13 +1862,13 @@
         <v>53</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
@@ -1860,7 +1879,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>2</v>
@@ -1875,7 +1894,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="8" t="s">
         <v>27</v>
       </c>
@@ -1886,7 +1905,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>2</v>
@@ -1901,7 +1920,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -1912,7 +1931,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>2</v>
@@ -1927,7 +1946,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -1938,7 +1957,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>2</v>
@@ -1953,7 +1972,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
@@ -1964,7 +1983,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>2</v>
@@ -1979,7 +1998,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
@@ -1990,7 +2009,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>2</v>
@@ -2005,7 +2024,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="8" t="s">
         <v>35</v>
       </c>
@@ -2016,7 +2035,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>2</v>
@@ -2031,7 +2050,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="8" t="s">
         <v>33</v>
       </c>
@@ -2042,7 +2061,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>2</v>
@@ -2057,7 +2076,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="8" t="s">
         <v>34</v>
       </c>
@@ -2068,7 +2087,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>2</v>
@@ -2083,7 +2102,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="8" t="s">
         <v>37</v>
       </c>
@@ -2094,7 +2113,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>2</v>
@@ -2109,7 +2128,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="8" t="s">
         <v>39</v>
       </c>
@@ -2120,7 +2139,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>2</v>
@@ -2135,7 +2154,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
@@ -2146,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>2</v>
@@ -2161,7 +2180,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="8" t="s">
         <v>16</v>
       </c>
@@ -2172,7 +2191,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>2</v>
@@ -2187,7 +2206,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
@@ -2198,7 +2217,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>2</v>
@@ -2213,7 +2232,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
@@ -2224,7 +2243,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>2</v>
@@ -2239,7 +2258,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="8" t="s">
         <v>24</v>
       </c>
@@ -2250,7 +2269,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>2</v>
@@ -2265,7 +2284,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
@@ -2276,7 +2295,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>2</v>
@@ -2291,226 +2310,224 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>87</v>
-      </c>
+    <row r="21" spans="1:8">
+      <c r="A21" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="10"/>
       <c r="G21" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>87</v>
+        <v>156</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>87</v>
+        <v>156</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>87</v>
+        <v>156</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>87</v>
+        <v>156</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>87</v>
+        <v>156</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>87</v>
+        <v>156</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>87</v>
+        <v>156</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="8" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>65</v>
+        <v>167</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>62</v>
@@ -2519,24 +2536,24 @@
         <v>63</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="8" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>62</v>
@@ -2545,24 +2562,24 @@
         <v>63</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="8" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>62</v>
@@ -2571,24 +2588,24 @@
         <v>63</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="8" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>62</v>
@@ -2597,24 +2614,24 @@
         <v>63</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="8" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>62</v>
@@ -2623,24 +2640,24 @@
         <v>63</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="8" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>62</v>
@@ -2649,24 +2666,24 @@
         <v>63</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>167</v>
+        <v>137</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>62</v>
@@ -2675,24 +2692,24 @@
         <v>63</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="8" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>62</v>
@@ -2701,50 +2718,50 @@
         <v>63</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>129</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E37" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="2" t="s">
         <v>63</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="8" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>62</v>
@@ -2753,302 +2770,302 @@
         <v>63</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="8" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>63</v>
+      <c r="F39" s="11" t="s">
+        <v>193</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="8" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="8" t="s">
-        <v>63</v>
+      <c r="F40" s="11" t="s">
+        <v>193</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>63</v>
+        <v>156</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>63</v>
+        <v>156</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>63</v>
+        <v>156</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>63</v>
+        <v>156</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>63</v>
+        <v>156</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>151</v>
+        <v>156</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>62</v>
+        <v>156</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>195</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>194</v>
+        <v>87</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="B49" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>87</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G157">
-    <sortCondition ref="E2:E157"/>
-    <sortCondition ref="F2:F157"/>
+  <sortState ref="A2:H49">
+    <sortCondition ref="E2:E49"/>
+    <sortCondition ref="F2:F49"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated to include references for Redondoviridae, Smacoviridae, among other lineages
</commit_message>
<xml_diff>
--- a/tabular/core/cress-refseqs-side-data.xlsx
+++ b/tabular/core/cress-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EA8F78-4F79-CC40-9FCD-B9EFAFAFB001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBBCF3A-8BFD-A645-AE0B-2E99F595722F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="1580" windowWidth="36380" windowHeight="20160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26720" yWindow="3760" windowWidth="21380" windowHeight="20400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="213">
   <si>
     <t>PCV-1</t>
   </si>
@@ -616,6 +616,57 @@
   </si>
   <si>
     <t>CRESS-2</t>
+  </si>
+  <si>
+    <t>MK059763</t>
+  </si>
+  <si>
+    <t>MF669476</t>
+  </si>
+  <si>
+    <t>KJ888053</t>
+  </si>
+  <si>
+    <t>MK059757</t>
+  </si>
+  <si>
+    <t>Brisavirus</t>
+  </si>
+  <si>
+    <t>Gemininvirus</t>
+  </si>
+  <si>
+    <t>Gemininviridae</t>
+  </si>
+  <si>
+    <t>Smacovirus</t>
+  </si>
+  <si>
+    <t>Vientovirus</t>
+  </si>
+  <si>
+    <t>HLVV</t>
+  </si>
+  <si>
+    <t>CBSV</t>
+  </si>
+  <si>
+    <t>EACMKV</t>
+  </si>
+  <si>
+    <t>L-BrV-RC</t>
+  </si>
+  <si>
+    <t>Human lung-associated brisavirus RC</t>
+  </si>
+  <si>
+    <t>East African cassava mosaic Kenya virus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cattle blood-associated circovirus-like virus </t>
+  </si>
+  <si>
+    <t>Human lung-associated vientovirus FB</t>
   </si>
 </sst>
 </file>
@@ -1778,10 +1829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G42" sqref="A1:H49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3068,6 +3119,110 @@
         <v>156</v>
       </c>
     </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H49">
     <sortCondition ref="E2:E49"/>

</xml_diff>

<commit_message>
Refactoring for new expanded root alignment
</commit_message>
<xml_diff>
--- a/tabular/core/cress-refseqs-side-data.xlsx
+++ b/tabular/core/cress-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBBCF3A-8BFD-A645-AE0B-2E99F595722F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668D638C-9AC9-3B4B-8A0F-322576ED851C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26720" yWindow="3760" windowWidth="21380" windowHeight="20400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="216">
   <si>
     <t>PCV-1</t>
   </si>
@@ -667,6 +667,15 @@
   </si>
   <si>
     <t>Human lung-associated vientovirus FB</t>
+  </si>
+  <si>
+    <t>Redondoviridae</t>
+  </si>
+  <si>
+    <t>Smacoviridae</t>
+  </si>
+  <si>
+    <t>Porprismacovirus</t>
   </si>
 </sst>
 </file>
@@ -1831,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:H53"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D49" sqref="A1:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3130,7 +3139,7 @@
         <v>212</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>204</v>
@@ -3156,10 +3165,10 @@
         <v>211</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>203</v>
@@ -3208,7 +3217,7 @@
         <v>209</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>200</v>

</xml_diff>

<commit_message>
Refactoring constrained alignment tree - more family-level branches
</commit_message>
<xml_diff>
--- a/tabular/core/cress-refseqs-side-data.xlsx
+++ b/tabular/core/cress-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668D638C-9AC9-3B4B-8A0F-322576ED851C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37983AF-1685-AF48-A2D5-BDE34F25215B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1840,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D49" sqref="A1:H53"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C47" sqref="A1:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2904,8 +2904,8 @@
       <c r="C41" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>192</v>
+      <c r="D41" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>194</v>
@@ -2930,8 +2930,8 @@
       <c r="C42" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>192</v>
+      <c r="D42" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>194</v>
@@ -2956,8 +2956,8 @@
       <c r="C43" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>192</v>
+      <c r="D43" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>194</v>
@@ -2982,8 +2982,8 @@
       <c r="C44" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>192</v>
+      <c r="D44" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>194</v>
@@ -3008,8 +3008,8 @@
       <c r="C45" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>192</v>
+      <c r="D45" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>194</v>
@@ -3034,8 +3034,8 @@
       <c r="C46" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>192</v>
+      <c r="D46" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>194</v>
@@ -3060,8 +3060,8 @@
       <c r="C47" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>192</v>
+      <c r="D47" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>194</v>
@@ -3086,8 +3086,8 @@
       <c r="C48" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>192</v>
+      <c r="D48" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>194</v>
@@ -3112,8 +3112,8 @@
       <c r="C49" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D49" s="8" t="s">
-        <v>192</v>
+      <c r="D49" s="11" t="s">
+        <v>195</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>195</v>

</xml_diff>

<commit_message>
Phylogeny build for core project
</commit_message>
<xml_diff>
--- a/tabular/core/cress-refseqs-side-data.xlsx
+++ b/tabular/core/cress-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33986C9A-779F-2E4B-8B35-D5B0E8F3C869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D519E4BF-F845-8E43-BB0E-E70B2CD47D51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4520" yWindow="3740" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="367">
   <si>
     <t>PCV-1</t>
   </si>
@@ -676,13 +676,466 @@
   </si>
   <si>
     <t>Porprismacovirus</t>
+  </si>
+  <si>
+    <t>NC_017916</t>
+  </si>
+  <si>
+    <t>NC_023887</t>
+  </si>
+  <si>
+    <t>NC_030120</t>
+  </si>
+  <si>
+    <t>NC_030122</t>
+  </si>
+  <si>
+    <t>NC_030121</t>
+  </si>
+  <si>
+    <t>NC_027777</t>
+  </si>
+  <si>
+    <t>NC_021203</t>
+  </si>
+  <si>
+    <t>NC_030127</t>
+  </si>
+  <si>
+    <t>NC_024774</t>
+  </si>
+  <si>
+    <t>NC_024775</t>
+  </si>
+  <si>
+    <t>NC_024773</t>
+  </si>
+  <si>
+    <t>NC_024776</t>
+  </si>
+  <si>
+    <t>NC_024772</t>
+  </si>
+  <si>
+    <t>NC_039071</t>
+  </si>
+  <si>
+    <t>NC_021204</t>
+  </si>
+  <si>
+    <t>NC_030126</t>
+  </si>
+  <si>
+    <t>NC_024119</t>
+  </si>
+  <si>
+    <t>NC_026320</t>
+  </si>
+  <si>
+    <t>NC_035474</t>
+  </si>
+  <si>
+    <t>NC_039070</t>
+  </si>
+  <si>
+    <t>NC_026318</t>
+  </si>
+  <si>
+    <t>NC_026317</t>
+  </si>
+  <si>
+    <t>NC_026319</t>
+  </si>
+  <si>
+    <t>NC_040336</t>
+  </si>
+  <si>
+    <t>NC_039069</t>
+  </si>
+  <si>
+    <t>NC_039068</t>
+  </si>
+  <si>
+    <t>NC_039067</t>
+  </si>
+  <si>
+    <t>NC_039066</t>
+  </si>
+  <si>
+    <t>NC_039065</t>
+  </si>
+  <si>
+    <t>NC_039064</t>
+  </si>
+  <si>
+    <t>NC_030119</t>
+  </si>
+  <si>
+    <t>NC_040359</t>
+  </si>
+  <si>
+    <t>NC_026252</t>
+  </si>
+  <si>
+    <t>NC_039063</t>
+  </si>
+  <si>
+    <t>NC_039062</t>
+  </si>
+  <si>
+    <t>NC_039061</t>
+  </si>
+  <si>
+    <t>NC_033275</t>
+  </si>
+  <si>
+    <t>NC_039060</t>
+  </si>
+  <si>
+    <t>NC_039059</t>
+  </si>
+  <si>
+    <t>NC_030129</t>
+  </si>
+  <si>
+    <t>NC_030124</t>
+  </si>
+  <si>
+    <t>NC_039058</t>
+  </si>
+  <si>
+    <t>NC_039057</t>
+  </si>
+  <si>
+    <t>NC_030125</t>
+  </si>
+  <si>
+    <t>NC_039056</t>
+  </si>
+  <si>
+    <t>NC_030128</t>
+  </si>
+  <si>
+    <t>NC_039055</t>
+  </si>
+  <si>
+    <t>NC_039054</t>
+  </si>
+  <si>
+    <t>NC_030123</t>
+  </si>
+  <si>
+    <t>Pig stool associated circular ssDNA virus GER2011</t>
+  </si>
+  <si>
+    <t>Turkey associated porprismacovirus 1</t>
+  </si>
+  <si>
+    <t>Sheep faeces associated smacovirus 3</t>
+  </si>
+  <si>
+    <t>Sheep faeces associated smacovirus 2</t>
+  </si>
+  <si>
+    <t>Sheep faeces associated smacovirus 1</t>
+  </si>
+  <si>
+    <t>Rat associated porprismacovirus 1</t>
+  </si>
+  <si>
+    <t>Porcine stool-associated circular virus 2</t>
+  </si>
+  <si>
+    <t>Porcine stool-associated circular virus</t>
+  </si>
+  <si>
+    <t>Porcine associated porprismacovirus 9</t>
+  </si>
+  <si>
+    <t>Porcine associated porprismacovirus 8</t>
+  </si>
+  <si>
+    <t>Porcine associated porprismacovirus 7</t>
+  </si>
+  <si>
+    <t>Porcine associated porprismacovirus 6</t>
+  </si>
+  <si>
+    <t>Porcine associated porprismacovirus 5</t>
+  </si>
+  <si>
+    <t>Porcine associated porprismacovirus 4</t>
+  </si>
+  <si>
+    <t>Porcine associated porprismacovirus 3</t>
+  </si>
+  <si>
+    <t>Porcine associated porprismacovirus 10</t>
+  </si>
+  <si>
+    <t>PoSCV Kor J481</t>
+  </si>
+  <si>
+    <t>Lemur associated porprismacovirus 1</t>
+  </si>
+  <si>
+    <t>Human feces smacovirus 3</t>
+  </si>
+  <si>
+    <t>Human feces smacovirus 2</t>
+  </si>
+  <si>
+    <t>Human associated porprismacovirus 2</t>
+  </si>
+  <si>
+    <t>Howler monkey associated porprismacovirus 1</t>
+  </si>
+  <si>
+    <t>Gorilla associated porprismacovirus 1</t>
+  </si>
+  <si>
+    <t>Fly associated circular virus 4</t>
+  </si>
+  <si>
+    <t>Chimpanzee associated porprismacovirus 2</t>
+  </si>
+  <si>
+    <t>Chimpanzee associated porprismacovirus 1</t>
+  </si>
+  <si>
+    <t>Camel associated porprismacovirus 4</t>
+  </si>
+  <si>
+    <t>Camel associated porprismacovirus 3</t>
+  </si>
+  <si>
+    <t>Camel associated porprismacovirus 2</t>
+  </si>
+  <si>
+    <t>Camel associated porprismacovirus 1</t>
+  </si>
+  <si>
+    <t>Bovine faeces associated smacovirus 2</t>
+  </si>
+  <si>
+    <t>Alces alces faeces associated smacovirus MP78</t>
+  </si>
+  <si>
+    <t>Human smacovirus 1</t>
+  </si>
+  <si>
+    <t>Human associated huchismacovirus 3</t>
+  </si>
+  <si>
+    <t>Human associated huchismacovirus 2</t>
+  </si>
+  <si>
+    <t>Human associated huchismacovirus 1</t>
+  </si>
+  <si>
+    <t>Chicken associated smacovirus</t>
+  </si>
+  <si>
+    <t>Chicken associated huchismacovirus 2</t>
+  </si>
+  <si>
+    <t>Chicken associated huchismacovirus 1</t>
+  </si>
+  <si>
+    <t>Bovine faeces associated smacovirus 6</t>
+  </si>
+  <si>
+    <t>Bovine faeces associated smacovirus 1</t>
+  </si>
+  <si>
+    <t>Camel associated drosmacovirus 2</t>
+  </si>
+  <si>
+    <t>Camel associated drosmacovirus 1</t>
+  </si>
+  <si>
+    <t>Bovine faeces associated smacovirus 5</t>
+  </si>
+  <si>
+    <t>Odonata-associated circular virus 5</t>
+  </si>
+  <si>
+    <t>Bovine faeces associated smacovirus 4</t>
+  </si>
+  <si>
+    <t>Odonata-associated circular virus 21</t>
+  </si>
+  <si>
+    <t>Circoviridae bovine stool/BK/KOR/2011</t>
+  </si>
+  <si>
+    <t>Bovine faeces associated smacovirus 3</t>
+  </si>
+  <si>
+    <t>Huchismacovirus</t>
+  </si>
+  <si>
+    <t>Drosmacovirus</t>
+  </si>
+  <si>
+    <t>Dragsmacovirus</t>
+  </si>
+  <si>
+    <t>Cosmacovirus</t>
+  </si>
+  <si>
+    <t>Bovismacovirus</t>
+  </si>
+  <si>
+    <t>PoSCV</t>
+  </si>
+  <si>
+    <t>PoSCV-10</t>
+  </si>
+  <si>
+    <t>PoSCV-3</t>
+  </si>
+  <si>
+    <t>PoSCV-4</t>
+  </si>
+  <si>
+    <t>PoSCV-5</t>
+  </si>
+  <si>
+    <t>PoSCV-6</t>
+  </si>
+  <si>
+    <t>PoSCV-7</t>
+  </si>
+  <si>
+    <t>PoSCV-8</t>
+  </si>
+  <si>
+    <t>PoSCV-9</t>
+  </si>
+  <si>
+    <t>GER2011</t>
+  </si>
+  <si>
+    <t>TaPSV</t>
+  </si>
+  <si>
+    <t>OvaPSV-3</t>
+  </si>
+  <si>
+    <t>OvaPSV-2</t>
+  </si>
+  <si>
+    <t>OvaPSV-1</t>
+  </si>
+  <si>
+    <t>RaaPSV-1</t>
+  </si>
+  <si>
+    <t>PoaPSV-2</t>
+  </si>
+  <si>
+    <t>PoaPSV</t>
+  </si>
+  <si>
+    <t>Camel-PoSCV-1</t>
+  </si>
+  <si>
+    <t>Camel-PoSCV-2</t>
+  </si>
+  <si>
+    <t>Camel-PoSCV-3</t>
+  </si>
+  <si>
+    <t>Camel-PoSCV-4</t>
+  </si>
+  <si>
+    <t>Chimp-PoSCV-1</t>
+  </si>
+  <si>
+    <t>Chimp-PoSCV-2</t>
+  </si>
+  <si>
+    <t>Human-PoSCV-2</t>
+  </si>
+  <si>
+    <t>Human-SCV-2</t>
+  </si>
+  <si>
+    <t>Lemur-PoSCV-1</t>
+  </si>
+  <si>
+    <t>HuchiSCV-1</t>
+  </si>
+  <si>
+    <t>HuchiSCV-2</t>
+  </si>
+  <si>
+    <t>HuchiSCV-3</t>
+  </si>
+  <si>
+    <t>Human-SCV-1</t>
+  </si>
+  <si>
+    <t>Alces-SCV</t>
+  </si>
+  <si>
+    <t>Bovine-SCV-2</t>
+  </si>
+  <si>
+    <t>Fly-SCV--1</t>
+  </si>
+  <si>
+    <t>Gorilla-SCV--1</t>
+  </si>
+  <si>
+    <t>Howler-SCV--1</t>
+  </si>
+  <si>
+    <t>Bovine-SCV-1</t>
+  </si>
+  <si>
+    <t>Bovine-SCV-6</t>
+  </si>
+  <si>
+    <t>Chicken-HuchiSCV-1</t>
+  </si>
+  <si>
+    <t>Chicken-HuchiSCV-2</t>
+  </si>
+  <si>
+    <t>Chicken-SCV</t>
+  </si>
+  <si>
+    <t>Camel-SCV-1</t>
+  </si>
+  <si>
+    <t>Camel-SCV-2</t>
+  </si>
+  <si>
+    <t>Bovine-SCV-4</t>
+  </si>
+  <si>
+    <t>Bovine-SCV-5</t>
+  </si>
+  <si>
+    <t>Odonata-CV-5</t>
+  </si>
+  <si>
+    <t>Bovine-SCV-3</t>
+  </si>
+  <si>
+    <t>Bovine-SCV</t>
+  </si>
+  <si>
+    <t>Odonata-CV-21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -735,6 +1188,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1158,7 +1618,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1177,6 +1637,7 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="330">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1845,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3163,22 +3624,22 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G51" s="11" t="s">
         <v>156</v>
@@ -3189,22 +3650,22 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>156</v>
@@ -3215,27 +3676,1301 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H62" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H70" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H73" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H75" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G76" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H76" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H77" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H78" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H79" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G80" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H80" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H81" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H82" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H83" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="H53" s="11" t="s">
+      <c r="C84" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H84" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H86" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H87" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H88" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H89" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H92" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H93" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H94" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H95" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H96" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G97" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H97" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G98" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H98" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H99" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H100" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H101" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G102" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H102" s="11" t="s">
         <v>156</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Root alignment update and tutorial web page update
</commit_message>
<xml_diff>
--- a/tabular/core/cress-refseqs-side-data.xlsx
+++ b/tabular/core/cress-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A766CFBA-EBFB-0B4F-A0D3-AA8E86831E18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7308B3E4-EB72-D44B-81B4-1CD692B45CE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25560" yWindow="10960" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>PCV-1</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Avon-Heatchote Estuary Associated Virus 13</t>
-  </si>
-  <si>
-    <t>CRESS</t>
   </si>
   <si>
     <t>Sus scrofa</t>
@@ -233,6 +230,18 @@
   </si>
   <si>
     <t>D-aGmydgV</t>
+  </si>
+  <si>
+    <t>JN857329</t>
+  </si>
+  <si>
+    <t>Circoviridae batCV-SC703</t>
+  </si>
+  <si>
+    <t>CRESS-4</t>
+  </si>
+  <si>
+    <t>batCV-Sc703</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1376,7 @@
   <dimension ref="A1:Y520"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1393,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -1393,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -1402,10 +1411,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -1419,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>2</v>
@@ -1428,10 +1437,10 @@
         <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -1453,28 +1462,28 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -1496,28 +1505,28 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -1539,28 +1548,28 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -1591,19 +1600,19 @@
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>13</v>
+      <c r="F6" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -1625,28 +1634,28 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1668,28 +1677,28 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -1711,28 +1720,28 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1754,28 +1763,28 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1797,28 +1806,28 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1840,28 +1849,28 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1883,28 +1892,28 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
@@ -1925,14 +1934,30 @@
       <c r="Y13"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
+      <c r="A14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>

</xml_diff>

<commit_message>
Expand master reference set
</commit_message>
<xml_diff>
--- a/tabular/core/cress-refseqs-side-data.xlsx
+++ b/tabular/core/cress-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE792A4-C264-0049-BA03-D356E64B7649}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6476C20-ECA0-1245-9B8F-087A4ABE76A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="7220" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1582,7 +1582,7 @@
   <dimension ref="A1:AA519"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="A1:J27"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactoring and adding Genomoviridae
</commit_message>
<xml_diff>
--- a/tabular/core/cress-refseqs-side-data.xlsx
+++ b/tabular/core/cress-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10ABDB9-5B96-CA4A-BD6E-398273430282}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFE4349-9E2A-D24A-A9DB-B39F3C83F976}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="7220" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,13 +427,13 @@
     <t>Protobacilladnavirus</t>
   </si>
   <si>
-    <t>superorder</t>
-  </si>
-  <si>
     <t>Arfiviricetes</t>
   </si>
   <si>
     <t>Repensiviricetes</t>
+  </si>
+  <si>
+    <t>class</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1582,7 @@
   <dimension ref="A1:AA519"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D5" sqref="A1:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1610,7 +1610,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>109</v>
@@ -1642,7 +1642,7 @@
         <v>120</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>124</v>
@@ -1691,7 +1691,7 @@
         <v>121</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>124</v>
@@ -1740,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>125</v>
@@ -1789,7 +1789,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>125</v>
@@ -1838,7 +1838,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>125</v>
@@ -1887,7 +1887,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>125</v>
@@ -1936,7 +1936,7 @@
         <v>67</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>125</v>
@@ -1985,7 +1985,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>126</v>
@@ -2034,7 +2034,7 @@
         <v>118</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>122</v>
@@ -2083,7 +2083,7 @@
         <v>117</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>122</v>
@@ -2132,7 +2132,7 @@
         <v>70</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>127</v>
@@ -2181,7 +2181,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>127</v>
@@ -2230,7 +2230,7 @@
         <v>81</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>128</v>
@@ -2279,7 +2279,7 @@
         <v>37</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>128</v>
@@ -2328,7 +2328,7 @@
         <v>83</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>128</v>
@@ -2377,7 +2377,7 @@
         <v>84</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>128</v>
@@ -2426,7 +2426,7 @@
         <v>85</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>128</v>
@@ -2475,7 +2475,7 @@
         <v>87</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>128</v>
@@ -2524,7 +2524,7 @@
         <v>86</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>128</v>
@@ -2573,7 +2573,7 @@
         <v>88</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>128</v>
@@ -2622,7 +2622,7 @@
         <v>89</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>128</v>
@@ -2671,7 +2671,7 @@
         <v>56</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>128</v>
@@ -2720,7 +2720,7 @@
         <v>60</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>128</v>
@@ -2769,7 +2769,7 @@
         <v>57</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>128</v>
@@ -2818,7 +2818,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>128</v>
@@ -2867,7 +2867,7 @@
         <v>59</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>128</v>

</xml_diff>